<commit_message>
Updated for "Additional Item Drops by Enemy".
</commit_message>
<xml_diff>
--- a/EnemySigilDrop.xlsx
+++ b/EnemySigilDrop.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="82">
   <si>
     <t>enemyName</t>
   </si>
@@ -26,61 +26,139 @@
     <t>drop[0].itemChance</t>
   </si>
   <si>
+    <t>drop[1].itemName</t>
+  </si>
+  <si>
+    <t>drop[1].itemDropChance</t>
+  </si>
+  <si>
+    <t>drop[1].itemChance</t>
+  </si>
+  <si>
+    <t>drop[2].itemName</t>
+  </si>
+  <si>
+    <t>drop[2].itemDropChance</t>
+  </si>
+  <si>
+    <t>drop[2].itemChance</t>
+  </si>
+  <si>
+    <t>drop[3].itemName</t>
+  </si>
+  <si>
+    <t>drop[3].itemDropChance</t>
+  </si>
+  <si>
+    <t>drop[3].itemChance</t>
+  </si>
+  <si>
+    <t>drop[4].itemName</t>
+  </si>
+  <si>
+    <t>drop[4].itemDropChance</t>
+  </si>
+  <si>
+    <t>drop[4].itemChance</t>
+  </si>
+  <si>
+    <t>drop[5].itemName</t>
+  </si>
+  <si>
+    <t>drop[5].itemDropChance</t>
+  </si>
+  <si>
+    <t>drop[5].itemChance</t>
+  </si>
+  <si>
+    <t>Exploiter Orb</t>
+  </si>
+  <si>
+    <t>Ecosynth Analyzer</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>0.1667</t>
+  </si>
+  <si>
+    <t>Entroplasma</t>
+  </si>
+  <si>
+    <t>Sagan Module</t>
+  </si>
+  <si>
+    <t>Lathe Coagulant</t>
+  </si>
+  <si>
+    <t>Zodian</t>
+  </si>
+  <si>
+    <t>Thyst</t>
+  </si>
+  <si>
+    <t>Corrupted Vor</t>
+  </si>
+  <si>
+    <t>Vor Sigil</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Hyena Pack</t>
+  </si>
+  <si>
+    <t>Hyena Sigil</t>
+  </si>
+  <si>
+    <t>Lephantis</t>
+  </si>
+  <si>
+    <t>Lephantis Sigil</t>
+  </si>
+  <si>
+    <t>Commander</t>
+  </si>
+  <si>
+    <t>Sargas Ruk Sigil</t>
+  </si>
+  <si>
+    <t>Infested Corpus</t>
+  </si>
+  <si>
+    <t>Raptor Mt</t>
+  </si>
+  <si>
+    <t>Raptor Sigil</t>
+  </si>
+  <si>
+    <t>General Sargas Ruk</t>
+  </si>
+  <si>
+    <t>Stalker</t>
+  </si>
+  <si>
+    <t>Stalker Sigil</t>
+  </si>
+  <si>
+    <t>Ambulas</t>
+  </si>
+  <si>
+    <t>Ambulas Sigil</t>
+  </si>
+  <si>
     <t>Raptor</t>
   </si>
   <si>
-    <t>Raptor Sigil</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>Corrupted Vor</t>
-  </si>
-  <si>
-    <t>Vor Sigil</t>
-  </si>
-  <si>
-    <t>Hyena Pack</t>
-  </si>
-  <si>
-    <t>Hyena Sigil</t>
-  </si>
-  <si>
-    <t>Lephantis</t>
-  </si>
-  <si>
-    <t>Lephantis Sigil</t>
-  </si>
-  <si>
-    <t>Commander</t>
-  </si>
-  <si>
-    <t>Sargas Ruk Sigil</t>
-  </si>
-  <si>
-    <t>Raptor Mt</t>
-  </si>
-  <si>
-    <t>Infested Corpus</t>
-  </si>
-  <si>
-    <t>General Sargas Ruk</t>
-  </si>
-  <si>
-    <t>Stalker</t>
-  </si>
-  <si>
-    <t>Stalker Sigil</t>
-  </si>
-  <si>
     <t>Hunhow</t>
   </si>
   <si>
-    <t>Ambulas</t>
-  </si>
-  <si>
-    <t>Ambulas Sigil</t>
+    <t>Lt Lech Kril</t>
+  </si>
+  <si>
+    <t>Lech Kril Sigil</t>
   </si>
   <si>
     <t>Tyl Regor</t>
@@ -89,12 +167,6 @@
     <t>Tyl Regor Sigil</t>
   </si>
   <si>
-    <t>Lt Lech Kril</t>
-  </si>
-  <si>
-    <t>Lech Kril Sigil</t>
-  </si>
-  <si>
     <t>Infested Grineer</t>
   </si>
   <si>
@@ -158,22 +230,22 @@
     <t>Zanuka Sigil</t>
   </si>
   <si>
+    <t>Vem Tabook</t>
+  </si>
+  <si>
+    <t>Grustrag Sigil</t>
+  </si>
+  <si>
     <t>Hyena Th</t>
   </si>
   <si>
-    <t>Vem Tabook</t>
-  </si>
-  <si>
-    <t>Grustrag Sigil</t>
+    <t>Councilor Vay Hek</t>
+  </si>
+  <si>
+    <t>Vay Hek Sigil</t>
   </si>
   <si>
     <t>Shadow Stalker</t>
-  </si>
-  <si>
-    <t>Councilor Vay Hek</t>
-  </si>
-  <si>
-    <t>Vay Hek Sigil</t>
   </si>
   <si>
     <t>Vay Hek Terra Frame</t>
@@ -230,7 +302,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -249,481 +321,585 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>